<commit_message>
new changes 28 aug
</commit_message>
<xml_diff>
--- a/ExcelSheet/amazontestdata.xlsx
+++ b/ExcelSheet/amazontestdata.xlsx
@@ -4,21 +4,28 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="16275" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14475" windowHeight="2475"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Samsung m32 128gb mobile</t>
+  </si>
+  <si>
+    <t>apple mobile 14 pro max</t>
+  </si>
+  <si>
+    <t>redmi note 12 pro plus 5g</t>
   </si>
 </sst>
 </file>
@@ -357,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -374,6 +381,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>